<commit_message>
v2.0 refactor the code.  divide the checkin.py to three part ( fileIO <-> backend <-> main).  fileIO.py handle the file IO with excel to create,read,update.  backend.py handle the checkIn system logic and commute with database(fileIO).  main.py now display the terminal view to let user use mode to contorl the checkin system
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="29005"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenjianyu/Desktop/CheckIn/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="account" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="2" r:id="rId2"/>
+    <sheet name="record" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
-  <si>
-    <t>座位</t>
-  </si>
-  <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>悠遊卡編號</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>checkInTime</t>
+  </si>
+  <si>
+    <t>checkOutTime</t>
   </si>
   <si>
     <t>1-1</t>
@@ -45,51 +34,57 @@
     <t>黑曜</t>
   </si>
   <si>
+    <t>2017-12-30 19:47:08</t>
+  </si>
+  <si>
     <t>1-2</t>
   </si>
   <si>
     <t>光秀</t>
   </si>
   <si>
+    <t>2017-12-30 19:47:41</t>
+  </si>
+  <si>
+    <t>2017-12-30 19:47:09</t>
+  </si>
+  <si>
     <t>1-3</t>
   </si>
   <si>
     <t>津沙</t>
   </si>
   <si>
+    <t>2017-12-30 19:47:37</t>
+  </si>
+  <si>
     <t>1-4</t>
   </si>
   <si>
     <t>鳥居</t>
   </si>
   <si>
+    <t>2017-12-30 19:47:13</t>
+  </si>
+  <si>
     <t>1-5</t>
   </si>
   <si>
     <t>廣鈕</t>
   </si>
   <si>
-    <t>簽到時間</t>
-  </si>
-  <si>
-    <t>簽退時間</t>
+    <t>2017-12-30 19:47:14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -118,20 +113,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -173,12 +163,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -205,15 +195,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -240,7 +229,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,16 +404,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,119 +421,69 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>